<commit_message>
The up-to-date Gantt Chart.
</commit_message>
<xml_diff>
--- a/Project_management/ip_sdi_gantt_chart__2_.xlsx
+++ b/Project_management/ip_sdi_gantt_chart__2_.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_nextcloud\00_kompaktkurs_projektmanangement\vorlagen\Gantt Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="363" documentId="11_4B07E0BD7483FB71D2FB3EEEBE287EAD8AE2B1E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B08E8F17-E6DC-4750-833F-D40801177747}"/>
+  <xr:revisionPtr revIDLastSave="370" documentId="11_4B07E0BD7483FB71D2FB3EEEBE287EAD8AE2B1E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A24C187-B54A-4A01-B5FC-B8B4748C2CA6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18348" windowHeight="8328" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,16 +143,16 @@
     <t>Decide on communication platform</t>
   </si>
   <si>
+    <t>Layout design</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Data integration</t>
+  </si>
+  <si>
     <t>Not started</t>
-  </si>
-  <si>
-    <t>Layout design</t>
-  </si>
-  <si>
-    <t>Metadata</t>
-  </si>
-  <si>
-    <t>Data integration</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -527,22 +527,22 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -949,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="25">
-        <v>0.35</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="30" customHeight="1">
@@ -1444,8 +1444,8 @@
         <f>D22-C22</f>
         <v>2</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>18</v>
+      <c r="F22" s="31" t="s">
+        <v>23</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="1"/>
@@ -1483,8 +1483,8 @@
         <f t="shared" ref="E23" si="0">D23-C23</f>
         <v>4</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>18</v>
+      <c r="F23" s="31" t="s">
+        <v>23</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="1"/>
@@ -1554,8 +1554,8 @@
         <f>D25-C25</f>
         <v>1</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>34</v>
+      <c r="F25" s="31" t="s">
+        <v>23</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="1"/>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="26" spans="1:24" ht="22.15" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>17</v>
@@ -1593,8 +1593,8 @@
         <f t="shared" ref="E26:E28" si="1">D26-C26</f>
         <v>7</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>34</v>
+      <c r="F26" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="1"/>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="27" spans="1:24" ht="22.15" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>20</v>
@@ -1632,8 +1632,8 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>34</v>
+      <c r="F27" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="1"/>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="28" spans="1:24" ht="22.15" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>20</v>
@@ -1672,7 +1672,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="1"/>
@@ -1743,7 +1743,7 @@
         <v>15</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="1"/>
@@ -1821,17 +1821,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E194172A664C3D44B55AD259CF5259CC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a3a3b985f66752244a6c0b9bb1957eb4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xmlns:ns3="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f1f5da211ee33ec20a81d51d442b62d" ns2:_="" ns3:_="">
     <xsd:import namespace="efe5fd09-895f-413c-ad62-8a7b7313e3f2"/>
@@ -2042,14 +2031,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{479041FF-5590-4492-B062-C11646B2FD6A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CA9E4B8-9B2B-4C88-B44A-6C68449E4F14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70DED035-8FC5-4FA4-AB9A-601E8E541F72}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70DED035-8FC5-4FA4-AB9A-601E8E541F72}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CA9E4B8-9B2B-4C88-B44A-6C68449E4F14}"/>
 </file>
</xml_diff>